<commit_message>
Modification of the ID3 algorithm and completion of the phasing of linguistic variables.
</commit_message>
<xml_diff>
--- a/DecisionTree/Resources/ExamplesAll.xlsx
+++ b/DecisionTree/Resources/ExamplesAll.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TechnicalProject14" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="190">
   <si>
     <t>Наблюдение</t>
   </si>
@@ -436,185 +436,164 @@
     <t>0.54</t>
   </si>
   <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>довольно высокий</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>довольно высокое</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>совсем плохая</t>
+  </si>
+  <si>
+    <t>совсем высокий</t>
+  </si>
+  <si>
+    <t>отличная</t>
+  </si>
+  <si>
+    <t>совсем низкое</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>довольно хороший</t>
+  </si>
+  <si>
+    <t>отличный</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>совсем низкий</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>0.39</t>
+  </si>
+  <si>
+    <t>довольно низкое</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>совсем хорошая</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>совсем высокое</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
     <t>1.54</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>довльно низкий</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>0.56</t>
-  </si>
-  <si>
-    <t>0.23</t>
-  </si>
-  <si>
-    <t>0.69</t>
-  </si>
-  <si>
-    <t>1.02</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>0.55</t>
-  </si>
-  <si>
-    <t>очень высокая</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>0.65</t>
-  </si>
-  <si>
-    <t>довольно высокий</t>
-  </si>
-  <si>
-    <t>0.91</t>
-  </si>
-  <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>1.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">высокий </t>
-  </si>
-  <si>
-    <t>довольно высокое</t>
-  </si>
-  <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>совсем плохая</t>
-  </si>
-  <si>
-    <t>совсем высокий</t>
-  </si>
-  <si>
-    <t>отличная</t>
-  </si>
-  <si>
-    <t>совсем низкое</t>
-  </si>
-  <si>
-    <t>0.50</t>
-  </si>
-  <si>
-    <t>довольно хороший</t>
-  </si>
-  <si>
-    <t>отличный</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>совсем низкий</t>
-  </si>
-  <si>
-    <t>0.88</t>
-  </si>
-  <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>0.39</t>
-  </si>
-  <si>
-    <t>довольно низкое</t>
-  </si>
-  <si>
-    <t>двольно низкое</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>совсем хорошая</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>1.23</t>
-  </si>
-  <si>
-    <t>0.49</t>
-  </si>
-  <si>
-    <t>0.37</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.31</t>
-  </si>
-  <si>
-    <t>совсем высокое</t>
-  </si>
-  <si>
-    <t>довльно высокое</t>
-  </si>
-  <si>
-    <t>0.32</t>
-  </si>
-  <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>0.87</t>
-  </si>
-  <si>
-    <t>0.41</t>
-  </si>
-  <si>
-    <t>0.90</t>
-  </si>
-  <si>
-    <t>0.35</t>
-  </si>
-  <si>
-    <t>0.59</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>0.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">очень высокое </t>
-  </si>
-  <si>
-    <t xml:space="preserve">высокое </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,6 +640,21 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -697,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -728,7 +722,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1034,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
@@ -1635,9 +1632,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,1983 +1667,1983 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="E7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C37" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D46" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="D48" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F50" s="13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="8" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C54" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D57" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="D62" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F62" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B63" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F71" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B75" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C75" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D78" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E78" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F81" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F82" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F90" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F94" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B95" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C95" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F95" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D97" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F98" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D99" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E99" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" s="13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="8" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C100" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="D100" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="E100" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F71" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F74" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F76" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D77" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E77" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="F77" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F78" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="F79" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F80" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F81" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F82" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F83" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F85" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F86" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E87" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F87" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C88" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F88" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D89" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F89" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E90" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F90" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E91" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F91" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C92" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F92" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D93" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F93" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="B94" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C94" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D94" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E94" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F94" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B95" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D95" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B96" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C96" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D96" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E96" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F96" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B97" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C97" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D97" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="E97" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F97" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E98" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F98" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B99" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C99" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D99" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E99" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F99" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B100" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C100" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D100" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E100" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F100" s="12" t="s">
+      <c r="F100" s="13" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>